<commit_message>
amplification and sequencing characteristics of usvi samples
</commit_message>
<xml_diff>
--- a/data/metadata/zika-usvi-sample-table.xlsx
+++ b/data/metadata/zika-usvi-sample-table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alliblk/Desktop/gitrepos/zika-usvi/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alliblk/Desktop/gitrepos/zika-usvi/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32000" yWindow="-5140" windowWidth="25600" windowHeight="15420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,8 +1007,9 @@
     <col min="1" max="1" width="10.1640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="15" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" style="6" customWidth="1"/>
-    <col min="4" max="6" width="10.5" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" style="6" customWidth="1"/>
+    <col min="4" max="5" width="10.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17" style="6" customWidth="1"/>
+    <col min="7" max="7" width="11" style="6" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" style="6" customWidth="1"/>
     <col min="9" max="9" width="13" style="6" customWidth="1"/>
     <col min="10" max="11" width="10.33203125" style="6" customWidth="1"/>

</xml_diff>